<commit_message>
parsing locales from xls
</commit_message>
<xml_diff>
--- a/sample_data/Sample_XLSX.xlsx
+++ b/sample_data/Sample_XLSX.xlsx
@@ -20,12 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en_US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fr_CA</t>
+  </si>
   <si>
     <t xml:space="preserve">simmple_string</t>
   </si>
   <si>
     <t xml:space="preserve">SimPle StiN G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple engliSH String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simPle US-En String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple-FR-cA String</t>
   </si>
 </sst>
 </file>
@@ -35,34 +59,58 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3465A4"/>
+        <bgColor rgb="FF3366FF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,8 +147,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -113,6 +169,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF3465A4"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -121,33 +237,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.94"/>
   </cols>
   <sheetData>
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
generating android folders structure for different locales
</commit_message>
<xml_diff>
--- a/sample_data/Sample_XLSX.xlsx
+++ b/sample_data/Sample_XLSX.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Default value</t>
+    <t xml:space="preserve">Default</t>
   </si>
   <si>
     <t xml:space="preserve">en</t>
@@ -240,10 +240,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.81"/>

</xml_diff>